<commit_message>
add npst class data; places/ folder; some documentation in resources; reorganize
</commit_message>
<xml_diff>
--- a/native_garden.xlsx
+++ b/native_garden.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisedgemon/repos/planting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chirs/repos/planting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2DFCEA-FD4B-6C45-8EFB-697958CD2718}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CAAD40-A3D8-5F46-BA4C-52F38035EF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="480" windowWidth="25440" windowHeight="14120" xr2:uid="{15BA4F13-2581-9841-A9DF-6B3D6C84267C}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14120" xr2:uid="{15BA4F13-2581-9841-A9DF-6B3D6C84267C}"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="1" r:id="rId1"/>
@@ -2224,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD367B52-4A65-FE4D-B97C-D9C08B69CC5F}">
   <dimension ref="A1:AB140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2336,7 +2336,7 @@
         <v>41</v>
       </c>
       <c r="G2" s="4">
-        <f>SUM(O2:W2)</f>
+        <f t="shared" ref="G2:G33" si="0">SUM(O2:W2)</f>
         <v>7</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -2358,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="Q2" s="4">
-        <f>IF(ISBLANK(Y2), "", 1)</f>
+        <f t="shared" ref="Q2:Q33" si="1">IF(ISBLANK(Y2), "", 1)</f>
         <v>1</v>
       </c>
       <c r="R2" s="4">
@@ -2391,7 +2391,7 @@
         <v>94</v>
       </c>
       <c r="G3" s="4">
-        <f>SUM(O3:W3)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -2413,7 +2413,7 @@
         <v>1</v>
       </c>
       <c r="Q3" s="4">
-        <f>IF(ISBLANK(Y3), "", 1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R3" s="4">
@@ -2446,7 +2446,7 @@
         <v>75</v>
       </c>
       <c r="G4" s="4">
-        <f>SUM(O4:W4)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -2471,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="Q4" s="4" t="str">
-        <f>IF(ISBLANK(Y4), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S4" s="4">
@@ -2504,7 +2504,7 @@
         <v>51</v>
       </c>
       <c r="G5" s="4">
-        <f>SUM(O5:W5)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -2526,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="Q5" s="4" t="str">
-        <f>IF(ISBLANK(Y5), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S5" s="4">
@@ -2556,7 +2556,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="4">
-        <f>SUM(O6:W6)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -2572,7 +2572,7 @@
         <v>57</v>
       </c>
       <c r="Q6" s="4" t="str">
-        <f>IF(ISBLANK(Y6), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R6" s="4">
@@ -2611,7 +2611,7 @@
         <v>88</v>
       </c>
       <c r="G7" s="4">
-        <f>SUM(O7:W7)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H7" s="4" t="s">
@@ -2633,7 +2633,7 @@
         <v>1</v>
       </c>
       <c r="Q7" s="4" t="str">
-        <f>IF(ISBLANK(Y7), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S7" s="4">
@@ -2666,7 +2666,7 @@
         <v>391</v>
       </c>
       <c r="G8" s="4">
-        <f>SUM(O8:W8)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H8" s="4" t="s">
@@ -2691,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="Q8" s="4" t="str">
-        <f>IF(ISBLANK(Y8), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R8" s="4">
@@ -2721,7 +2721,7 @@
         <v>71</v>
       </c>
       <c r="G9" s="4">
-        <f>SUM(O9:W9)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H9" s="4" t="s">
@@ -2740,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="Q9" s="4" t="str">
-        <f>IF(ISBLANK(Y9), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S9" s="4">
@@ -2773,7 +2773,7 @@
         <v>163</v>
       </c>
       <c r="G10" s="4">
-        <f>SUM(O10:W10)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H10" s="4" t="s">
@@ -2795,7 +2795,7 @@
         <v>1</v>
       </c>
       <c r="Q10" s="4" t="str">
-        <f>IF(ISBLANK(Y10), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U10" s="4">
@@ -2825,7 +2825,7 @@
         <v>143</v>
       </c>
       <c r="G11" s="4">
-        <f>SUM(O11:W11)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H11" s="4" t="s">
@@ -2841,7 +2841,7 @@
         <v>393</v>
       </c>
       <c r="Q11" s="4" t="str">
-        <f>IF(ISBLANK(Y11), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R11" s="4">
@@ -2874,7 +2874,7 @@
         <v>138</v>
       </c>
       <c r="G12" s="4">
-        <f>SUM(O12:W12)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H12" s="4" t="s">
@@ -2890,7 +2890,7 @@
         <v>393</v>
       </c>
       <c r="Q12" s="4">
-        <f>IF(ISBLANK(Y12), "", 1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R12" s="4">
@@ -2923,7 +2923,7 @@
         <v>74</v>
       </c>
       <c r="G13" s="4">
-        <f>SUM(O13:W13)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -2945,7 +2945,7 @@
         <v>1</v>
       </c>
       <c r="Q13" s="4" t="str">
-        <f>IF(ISBLANK(Y13), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S13" s="4">
@@ -2972,7 +2972,7 @@
         <v>141</v>
       </c>
       <c r="G14" s="4">
-        <f>SUM(O14:W14)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H14" s="4" t="s">
@@ -2988,7 +2988,7 @@
         <v>56</v>
       </c>
       <c r="Q14" s="4" t="str">
-        <f>IF(ISBLANK(Y14), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R14" s="4">
@@ -3018,7 +3018,7 @@
         <v>369</v>
       </c>
       <c r="G15" s="4">
-        <f>SUM(O15:W15)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -3034,7 +3034,7 @@
         <v>56</v>
       </c>
       <c r="Q15" s="4" t="str">
-        <f>IF(ISBLANK(Y15), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R15" s="4">
@@ -3067,7 +3067,7 @@
         <v>80</v>
       </c>
       <c r="G16" s="4">
-        <f>SUM(O16:W16)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H16" s="4" t="s">
@@ -3085,7 +3085,7 @@
       <c r="N16" s="4"/>
       <c r="O16" s="8"/>
       <c r="Q16" s="4" t="str">
-        <f>IF(ISBLANK(Y16), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S16" s="4">
@@ -3115,7 +3115,7 @@
         <v>62</v>
       </c>
       <c r="G17" s="4">
-        <f>SUM(O17:W17)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H17" s="4" t="s">
@@ -3134,7 +3134,7 @@
         <v>528</v>
       </c>
       <c r="Q17" s="4" t="str">
-        <f>IF(ISBLANK(Y17), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S17" s="4">
@@ -3167,7 +3167,7 @@
         <v>136</v>
       </c>
       <c r="G18" s="4">
-        <f>SUM(O18:W18)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H18" s="4" t="s">
@@ -3186,7 +3186,7 @@
         <v>1</v>
       </c>
       <c r="Q18" s="4" t="str">
-        <f>IF(ISBLANK(Y18), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R18" s="4">
@@ -3213,7 +3213,7 @@
         <v>46</v>
       </c>
       <c r="G19" s="4">
-        <f>SUM(O19:W19)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -3232,7 +3232,7 @@
         <v>1</v>
       </c>
       <c r="Q19" s="4" t="str">
-        <f>IF(ISBLANK(Y19), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S19" s="4">
@@ -3262,7 +3262,7 @@
         <v>68</v>
       </c>
       <c r="G20" s="4">
-        <f>SUM(O20:W20)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H20" s="4" t="s">
@@ -3278,7 +3278,7 @@
         <v>393</v>
       </c>
       <c r="Q20" s="4" t="str">
-        <f>IF(ISBLANK(Y20), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R20" s="4">
@@ -3311,7 +3311,7 @@
         <v>161</v>
       </c>
       <c r="G21" s="4">
-        <f>SUM(O21:W21)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H21" s="4" t="s">
@@ -3330,7 +3330,7 @@
         <v>-1</v>
       </c>
       <c r="Q21" s="4" t="str">
-        <f>IF(ISBLANK(Y21), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R21" s="4">
@@ -3366,7 +3366,7 @@
         <v>224</v>
       </c>
       <c r="G22" s="4">
-        <f>SUM(O22:W22)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H22" s="4" t="s">
@@ -3385,7 +3385,7 @@
         <v>1</v>
       </c>
       <c r="Q22" s="4">
-        <f>IF(ISBLANK(Y22), "", 1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="S22" s="4">
@@ -3412,7 +3412,7 @@
         <v>175</v>
       </c>
       <c r="G23" s="4">
-        <f>SUM(O23:W23)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H23" s="4" t="s">
@@ -3431,7 +3431,7 @@
         <v>1</v>
       </c>
       <c r="Q23" s="4" t="str">
-        <f>IF(ISBLANK(Y23), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R23" s="4">
@@ -3461,7 +3461,7 @@
         <v>154</v>
       </c>
       <c r="G24" s="4">
-        <f>SUM(O24:W24)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H24" s="4" t="s">
@@ -3483,7 +3483,7 @@
         <v>1</v>
       </c>
       <c r="Q24" s="4" t="str">
-        <f>IF(ISBLANK(Y24), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="V24" s="4">
@@ -3507,7 +3507,7 @@
         <v>182</v>
       </c>
       <c r="G25" s="4">
-        <f>SUM(O25:W25)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H25" s="4" t="s">
@@ -3526,7 +3526,7 @@
         <v>1</v>
       </c>
       <c r="Q25" s="4" t="str">
-        <f>IF(ISBLANK(Y25), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R25" s="4">
@@ -3553,7 +3553,7 @@
         <v>151</v>
       </c>
       <c r="G26" s="4">
-        <f>SUM(O26:W26)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H26" s="4" t="s">
@@ -3572,7 +3572,7 @@
         <v>1</v>
       </c>
       <c r="Q26" s="4" t="str">
-        <f>IF(ISBLANK(Y26), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R26" s="4">
@@ -3602,7 +3602,7 @@
         <v>531</v>
       </c>
       <c r="G27" s="4">
-        <f>SUM(O27:W27)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H27" s="4" t="s">
@@ -3621,7 +3621,7 @@
         <v>1</v>
       </c>
       <c r="Q27" s="4" t="str">
-        <f>IF(ISBLANK(Y27), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S27" s="4">
@@ -3651,7 +3651,7 @@
         <v>447</v>
       </c>
       <c r="G28" s="4">
-        <f>SUM(O28:W28)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H28" s="4" t="s">
@@ -3667,7 +3667,7 @@
         <v>57</v>
       </c>
       <c r="Q28" s="4" t="str">
-        <f>IF(ISBLANK(Y28), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="U28" s="4">
@@ -3697,7 +3697,7 @@
         <v>529</v>
       </c>
       <c r="G29" s="4">
-        <f>SUM(O29:W29)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H29" s="4" t="s">
@@ -3719,7 +3719,7 @@
         <v>1</v>
       </c>
       <c r="Q29" s="4">
-        <f>IF(ISBLANK(Y29), "", 1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="U29" s="4">
@@ -3746,7 +3746,7 @@
         <v>43</v>
       </c>
       <c r="G30" s="4">
-        <f>SUM(O30:W30)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H30" s="4" t="s">
@@ -3762,7 +3762,7 @@
         <v>57</v>
       </c>
       <c r="Q30" s="4" t="str">
-        <f>IF(ISBLANK(Y30), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T30" s="4">
@@ -3792,7 +3792,7 @@
         <v>401</v>
       </c>
       <c r="G31" s="4">
-        <f>SUM(O31:W31)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H31" s="4" t="s">
@@ -3808,7 +3808,7 @@
         <v>57</v>
       </c>
       <c r="Q31" s="4" t="str">
-        <f>IF(ISBLANK(Y31), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R31" s="4">
@@ -3838,7 +3838,7 @@
         <v>132</v>
       </c>
       <c r="G32" s="4">
-        <f>SUM(O32:W32)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H32" s="4" t="s">
@@ -3854,7 +3854,7 @@
         <v>56</v>
       </c>
       <c r="Q32" s="4" t="str">
-        <f>IF(ISBLANK(Y32), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S32" s="4">
@@ -3884,7 +3884,7 @@
         <v>436</v>
       </c>
       <c r="G33" s="4">
-        <f>SUM(O33:W33)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H33" s="4" t="s">
@@ -3900,7 +3900,7 @@
         <v>56</v>
       </c>
       <c r="Q33" s="4" t="str">
-        <f>IF(ISBLANK(Y33), "", 1)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="R33" s="4">
@@ -3927,7 +3927,7 @@
         <v>473</v>
       </c>
       <c r="G34" s="4">
-        <f>SUM(O34:W34)</f>
+        <f t="shared" ref="G34:G65" si="2">SUM(O34:W34)</f>
         <v>3</v>
       </c>
       <c r="H34" s="4" t="s">
@@ -3943,7 +3943,7 @@
         <v>56</v>
       </c>
       <c r="Q34" s="4" t="str">
-        <f>IF(ISBLANK(Y34), "", 1)</f>
+        <f t="shared" ref="Q34:Q65" si="3">IF(ISBLANK(Y34), "", 1)</f>
         <v/>
       </c>
       <c r="S34" s="4">
@@ -3973,7 +3973,7 @@
         <v>189</v>
       </c>
       <c r="G35" s="4">
-        <f>SUM(O35:W35)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H35" s="4" t="s">
@@ -3992,7 +3992,7 @@
         <v>1</v>
       </c>
       <c r="Q35" s="4" t="str">
-        <f>IF(ISBLANK(Y35), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="R35" s="4">
@@ -4016,7 +4016,7 @@
         <v>115</v>
       </c>
       <c r="G36" s="4">
-        <f>SUM(O36:W36)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H36" s="4" t="s">
@@ -4035,7 +4035,7 @@
         <v>-1</v>
       </c>
       <c r="Q36" s="4" t="str">
-        <f>IF(ISBLANK(Y36), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S36" s="4">
@@ -4068,7 +4068,7 @@
         <v>522</v>
       </c>
       <c r="G37" s="4">
-        <f>SUM(O37:W37)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H37" s="4" t="s">
@@ -4093,7 +4093,7 @@
         <v>1</v>
       </c>
       <c r="Q37" s="4" t="str">
-        <f>IF(ISBLANK(Y37), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S37" s="4">
@@ -4120,7 +4120,7 @@
         <v>280</v>
       </c>
       <c r="G38" s="4">
-        <f>SUM(O38:W38)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H38" s="4" t="s">
@@ -4139,7 +4139,7 @@
         <v>1</v>
       </c>
       <c r="Q38" s="4" t="str">
-        <f>IF(ISBLANK(Y38), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="R38" s="4">
@@ -4163,7 +4163,7 @@
         <v>180</v>
       </c>
       <c r="G39" s="4">
-        <f>SUM(O39:W39)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H39" s="4" t="s">
@@ -4182,7 +4182,7 @@
         <v>1</v>
       </c>
       <c r="Q39" s="4" t="str">
-        <f>IF(ISBLANK(Y39), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="R39" s="4">
@@ -4209,7 +4209,7 @@
         <v>463</v>
       </c>
       <c r="G40" s="4">
-        <f>SUM(O40:W40)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H40" s="4" t="s">
@@ -4228,7 +4228,7 @@
         <v>1</v>
       </c>
       <c r="Q40" s="4" t="str">
-        <f>IF(ISBLANK(Y40), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="U40" s="4">
@@ -4255,7 +4255,7 @@
         <v>466</v>
       </c>
       <c r="G41" s="4">
-        <f>SUM(O41:W41)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H41" s="4" t="s">
@@ -4274,7 +4274,7 @@
         <v>1</v>
       </c>
       <c r="Q41" s="4" t="str">
-        <f>IF(ISBLANK(Y41), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="T41" s="4">
@@ -4301,7 +4301,7 @@
         <v>321</v>
       </c>
       <c r="G42" s="4">
-        <f>SUM(O42:W42)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H42" s="4" t="s">
@@ -4320,7 +4320,7 @@
         <v>1</v>
       </c>
       <c r="Q42" s="4" t="str">
-        <f>IF(ISBLANK(Y42), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="U42" s="4">
@@ -4347,7 +4347,7 @@
         <v>419</v>
       </c>
       <c r="G43" s="4">
-        <f>SUM(O43:W43)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H43" s="4" t="s">
@@ -4366,7 +4366,7 @@
         <v>1</v>
       </c>
       <c r="Q43" s="4" t="str">
-        <f>IF(ISBLANK(Y43), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S43" s="4">
@@ -4393,7 +4393,7 @@
         <v>32</v>
       </c>
       <c r="G44" s="4">
-        <f>SUM(O44:W44)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H44" s="4" t="s">
@@ -4415,7 +4415,7 @@
         <v>1</v>
       </c>
       <c r="Q44" s="4" t="str">
-        <f>IF(ISBLANK(Y44), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="U44" s="4">
@@ -4442,7 +4442,7 @@
         <v>85</v>
       </c>
       <c r="G45" s="4">
-        <f>SUM(O45:W45)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H45" s="4" t="s">
@@ -4467,7 +4467,7 @@
         <v>1</v>
       </c>
       <c r="Q45" s="4" t="str">
-        <f>IF(ISBLANK(Y45), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="V45" s="4">
@@ -4491,7 +4491,7 @@
         <v>36</v>
       </c>
       <c r="G46" s="4">
-        <f>SUM(O46:W46)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H46" s="4" t="s">
@@ -4510,7 +4510,7 @@
         <v>1</v>
       </c>
       <c r="Q46" s="4" t="str">
-        <f>IF(ISBLANK(Y46), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="R46" s="4">
@@ -4537,7 +4537,7 @@
         <v>70</v>
       </c>
       <c r="G47" s="4">
-        <f>SUM(O47:W47)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H47" s="4" t="s">
@@ -4556,7 +4556,7 @@
         <v>393</v>
       </c>
       <c r="Q47" s="4" t="str">
-        <f>IF(ISBLANK(Y47), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S47" s="4">
@@ -4586,7 +4586,7 @@
         <v>525</v>
       </c>
       <c r="G48" s="4">
-        <f>SUM(O48:W48)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H48" s="4" t="s">
@@ -4608,7 +4608,7 @@
         <v>1</v>
       </c>
       <c r="Q48" s="4" t="str">
-        <f>IF(ISBLANK(Y48), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S48" s="4">
@@ -4632,7 +4632,7 @@
         <v>172</v>
       </c>
       <c r="G49" s="4">
-        <f>SUM(O49:W49)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H49" s="4" t="s">
@@ -4651,7 +4651,7 @@
         <v>-1</v>
       </c>
       <c r="Q49" s="4" t="str">
-        <f>IF(ISBLANK(Y49), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="R49" s="4">
@@ -4684,7 +4684,7 @@
         <v>530</v>
       </c>
       <c r="G50" s="4">
-        <f>SUM(O50:W50)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="H50" s="4" t="s">
@@ -4700,7 +4700,7 @@
         <v>399</v>
       </c>
       <c r="Q50" s="4" t="str">
-        <f>IF(ISBLANK(Y50), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S50" s="4">
@@ -4727,7 +4727,7 @@
         <v>187</v>
       </c>
       <c r="G51" s="4">
-        <f>SUM(O51:W51)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H51" s="4" t="s">
@@ -4743,7 +4743,7 @@
         <v>57</v>
       </c>
       <c r="Q51" s="4" t="str">
-        <f>IF(ISBLANK(Y51), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="R51" s="4">
@@ -4770,7 +4770,7 @@
         <v>315</v>
       </c>
       <c r="G52" s="4">
-        <f>SUM(O52:W52)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H52" s="4" t="s">
@@ -4786,7 +4786,7 @@
         <v>57</v>
       </c>
       <c r="Q52" s="4" t="str">
-        <f>IF(ISBLANK(Y52), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S52" s="4">
@@ -4810,7 +4810,7 @@
         <v>155</v>
       </c>
       <c r="G53" s="4">
-        <f>SUM(O53:W53)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H53" s="4" t="s">
@@ -4826,7 +4826,7 @@
         <v>57</v>
       </c>
       <c r="Q53" s="4" t="str">
-        <f>IF(ISBLANK(Y53), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="R53" s="4">
@@ -4853,7 +4853,7 @@
         <v>469</v>
       </c>
       <c r="G54" s="4">
-        <f>SUM(O54:W54)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H54" s="4" t="s">
@@ -4872,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="Q54" s="4" t="str">
-        <f>IF(ISBLANK(Y54), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="U54" s="4">
@@ -4896,7 +4896,7 @@
         <v>158</v>
       </c>
       <c r="G55" s="4">
-        <f>SUM(O55:W55)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H55" s="4" t="s">
@@ -4912,7 +4912,7 @@
         <v>1</v>
       </c>
       <c r="Q55" s="4" t="str">
-        <f>IF(ISBLANK(Y55), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="W55" s="4">
@@ -4933,7 +4933,7 @@
         <v>72</v>
       </c>
       <c r="G56" s="4">
-        <f>SUM(O56:W56)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H56" s="4" t="s">
@@ -4946,7 +4946,7 @@
         <v>57</v>
       </c>
       <c r="Q56" s="4" t="str">
-        <f>IF(ISBLANK(Y56), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S56" s="4">
@@ -4973,7 +4973,7 @@
         <v>446</v>
       </c>
       <c r="G57" s="4">
-        <f>SUM(O57:W57)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H57" s="4" t="s">
@@ -4992,7 +4992,7 @@
         <v>1</v>
       </c>
       <c r="Q57" s="4" t="str">
-        <f>IF(ISBLANK(Y57), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="T57" s="4">
@@ -5016,7 +5016,7 @@
         <v>285</v>
       </c>
       <c r="G58" s="4">
-        <f>SUM(O58:W58)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H58" s="4" t="s">
@@ -5035,7 +5035,7 @@
         <v>1</v>
       </c>
       <c r="Q58" s="4" t="str">
-        <f>IF(ISBLANK(Y58), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="R58" s="4">
@@ -5056,7 +5056,7 @@
         <v>400</v>
       </c>
       <c r="G59" s="4">
-        <f>SUM(O59:W59)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H59" s="4" t="s">
@@ -5069,7 +5069,7 @@
         <v>1</v>
       </c>
       <c r="Q59" s="4">
-        <f>IF(ISBLANK(Y59), "", 1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Y59" t="s">
@@ -5090,7 +5090,7 @@
         <v>170</v>
       </c>
       <c r="G60" s="4">
-        <f>SUM(O60:W60)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H60" s="4" t="s">
@@ -5106,7 +5106,7 @@
         <v>56</v>
       </c>
       <c r="Q60" s="4" t="str">
-        <f>IF(ISBLANK(Y60), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="R60" s="4">
@@ -5130,7 +5130,7 @@
         <v>471</v>
       </c>
       <c r="G61" s="4">
-        <f>SUM(O61:W61)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H61" s="4" t="s">
@@ -5149,7 +5149,7 @@
         <v>1</v>
       </c>
       <c r="Q61" s="4" t="str">
-        <f>IF(ISBLANK(Y61), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="U61" s="4">
@@ -5173,7 +5173,7 @@
         <v>443</v>
       </c>
       <c r="G62" s="4">
-        <f>SUM(O62:W62)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H62" s="4" t="s">
@@ -5192,7 +5192,7 @@
         <v>1</v>
       </c>
       <c r="Q62" s="4" t="str">
-        <f>IF(ISBLANK(Y62), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="T62" s="4">
@@ -5213,7 +5213,7 @@
         <v>349</v>
       </c>
       <c r="G63" s="4">
-        <f>SUM(O63:W63)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H63" s="4" t="s">
@@ -5229,7 +5229,7 @@
         <v>56</v>
       </c>
       <c r="Q63" s="4" t="str">
-        <f>IF(ISBLANK(Y63), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="R63" s="4">
@@ -5256,7 +5256,7 @@
         <v>109</v>
       </c>
       <c r="G64" s="4">
-        <f>SUM(O64:W64)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H64" s="4" t="s">
@@ -5275,7 +5275,7 @@
         <v>1</v>
       </c>
       <c r="Q64" s="4" t="str">
-        <f>IF(ISBLANK(Y64), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="W64" s="4">
@@ -5299,7 +5299,7 @@
         <v>99</v>
       </c>
       <c r="G65" s="4">
-        <f>SUM(O65:W65)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H65" s="4" t="s">
@@ -5315,7 +5315,7 @@
         <v>56</v>
       </c>
       <c r="Q65" s="4" t="str">
-        <f>IF(ISBLANK(Y65), "", 1)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S65" s="4">
@@ -5342,7 +5342,7 @@
         <v>449</v>
       </c>
       <c r="G66" s="4">
-        <f>SUM(O66:W66)</f>
+        <f t="shared" ref="G66:G97" si="4">SUM(O66:W66)</f>
         <v>2</v>
       </c>
       <c r="H66" s="4" t="s">
@@ -5352,7 +5352,7 @@
         <v>56</v>
       </c>
       <c r="Q66" s="4" t="str">
-        <f>IF(ISBLANK(Y66), "", 1)</f>
+        <f t="shared" ref="Q66:Q97" si="5">IF(ISBLANK(Y66), "", 1)</f>
         <v/>
       </c>
       <c r="R66" s="4">
@@ -5376,7 +5376,7 @@
         <v>247</v>
       </c>
       <c r="G67" s="4">
-        <f>SUM(O67:W67)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H67" s="4" t="s">
@@ -5398,7 +5398,7 @@
         <v>1</v>
       </c>
       <c r="Q67" s="4" t="str">
-        <f>IF(ISBLANK(Y67), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -5419,7 +5419,7 @@
         <v>412</v>
       </c>
       <c r="G68" s="4">
-        <f>SUM(O68:W68)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H68" s="4" t="s">
@@ -5438,7 +5438,7 @@
         <v>1</v>
       </c>
       <c r="Q68" s="4" t="str">
-        <f>IF(ISBLANK(Y68), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S68" s="4">
@@ -5459,7 +5459,7 @@
         <v>118</v>
       </c>
       <c r="G69" s="4">
-        <f>SUM(O69:W69)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H69" s="4" t="s">
@@ -5478,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="Q69" s="4" t="str">
-        <f>IF(ISBLANK(Y69), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="W69" s="4">
@@ -5502,7 +5502,7 @@
         <v>370</v>
       </c>
       <c r="G70" s="4">
-        <f>SUM(O70:W70)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H70" s="4" t="s">
@@ -5518,7 +5518,7 @@
         <v>393</v>
       </c>
       <c r="Q70" s="4" t="str">
-        <f>IF(ISBLANK(Y70), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="R70" s="4">
@@ -5542,7 +5542,7 @@
         <v>482</v>
       </c>
       <c r="G71" s="4">
-        <f>SUM(O71:W71)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H71" s="4" t="s">
@@ -5561,7 +5561,7 @@
         <v>1</v>
       </c>
       <c r="Q71" s="4" t="str">
-        <f>IF(ISBLANK(Y71), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="U71" s="4">
@@ -5585,7 +5585,7 @@
         <v>445</v>
       </c>
       <c r="G72" s="4">
-        <f>SUM(O72:W72)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H72" s="4" t="s">
@@ -5604,7 +5604,7 @@
         <v>1</v>
       </c>
       <c r="Q72" s="4" t="str">
-        <f>IF(ISBLANK(Y72), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T72" s="4">
@@ -5628,7 +5628,7 @@
         <v>222</v>
       </c>
       <c r="G73" s="4">
-        <f>SUM(O73:W73)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="H73" s="4" t="s">
@@ -5644,7 +5644,7 @@
         <v>399</v>
       </c>
       <c r="Q73" s="4" t="str">
-        <f>IF(ISBLANK(Y73), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T73" s="4">
@@ -5668,11 +5668,11 @@
         <v>365</v>
       </c>
       <c r="G74" s="4">
-        <f>SUM(O74:W74)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="Q74" s="4" t="str">
-        <f>IF(ISBLANK(Y74), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="R74" s="4">
@@ -5699,7 +5699,7 @@
         <v>232</v>
       </c>
       <c r="G75" s="4">
-        <f>SUM(O75:W75)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H75" s="4" t="s">
@@ -5715,7 +5715,7 @@
         <v>402</v>
       </c>
       <c r="Q75" s="4" t="str">
-        <f>IF(ISBLANK(Y75), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T75" s="4">
@@ -5736,7 +5736,7 @@
         <v>414</v>
       </c>
       <c r="G76" s="4">
-        <f>SUM(O76:W76)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H76" s="4" t="s">
@@ -5752,7 +5752,7 @@
         <v>56</v>
       </c>
       <c r="Q76" s="4" t="str">
-        <f>IF(ISBLANK(Y76), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S76" s="4">
@@ -5776,7 +5776,7 @@
         <v>459</v>
       </c>
       <c r="G77" s="4">
-        <f>SUM(O77:W77)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H77" s="4" t="s">
@@ -5792,7 +5792,7 @@
         <v>56</v>
       </c>
       <c r="Q77" s="4" t="str">
-        <f>IF(ISBLANK(Y77), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T77" s="4">
@@ -5813,7 +5813,7 @@
         <v>277</v>
       </c>
       <c r="G78" s="4">
-        <f>SUM(O78:W78)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H78" s="4" t="s">
@@ -5832,7 +5832,7 @@
         <v>1</v>
       </c>
       <c r="Q78" s="4" t="str">
-        <f>IF(ISBLANK(Y78), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -5850,11 +5850,11 @@
         <v>359</v>
       </c>
       <c r="G79" s="4">
-        <f>SUM(O79:W79)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q79" s="4" t="str">
-        <f>IF(ISBLANK(Y79), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="V79" s="4">
@@ -5875,11 +5875,11 @@
         <v>357</v>
       </c>
       <c r="G80" s="4">
-        <f>SUM(O80:W80)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q80" s="4" t="str">
-        <f>IF(ISBLANK(Y80), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="R80" s="4">
@@ -5900,11 +5900,11 @@
         <v>355</v>
       </c>
       <c r="G81" s="4">
-        <f>SUM(O81:W81)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q81" s="4" t="str">
-        <f>IF(ISBLANK(Y81), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="R81" s="4">
@@ -5925,11 +5925,11 @@
         <v>139</v>
       </c>
       <c r="G82" s="4">
-        <f>SUM(O82:W82)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q82" s="4" t="str">
-        <f>IF(ISBLANK(Y82), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="W82" s="4">
@@ -5953,11 +5953,11 @@
         <v>240</v>
       </c>
       <c r="G83" s="4">
-        <f>SUM(O83:W83)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q83" s="4" t="str">
-        <f>IF(ISBLANK(Y83), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T83" s="4">
@@ -5981,11 +5981,11 @@
         <v>212</v>
       </c>
       <c r="G84" s="4">
-        <f>SUM(O84:W84)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q84" s="4" t="str">
-        <f>IF(ISBLANK(Y84), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T84" s="4">
@@ -6009,11 +6009,11 @@
         <v>259</v>
       </c>
       <c r="G85" s="4">
-        <f>SUM(O85:W85)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q85" s="4" t="str">
-        <f>IF(ISBLANK(Y85), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T85" s="4">
@@ -6034,11 +6034,11 @@
         <v>378</v>
       </c>
       <c r="G86" s="4">
-        <f>SUM(O86:W86)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q86" s="4" t="str">
-        <f>IF(ISBLANK(Y86), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T86" s="4">
@@ -6059,14 +6059,14 @@
         <v>290</v>
       </c>
       <c r="G87" s="4">
-        <f>SUM(O87:W87)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O87" s="4">
         <v>1</v>
       </c>
       <c r="Q87" s="4" t="str">
-        <f>IF(ISBLANK(Y87), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -6084,14 +6084,14 @@
         <v>265</v>
       </c>
       <c r="G88" s="4">
-        <f>SUM(O88:W88)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P88" s="4">
         <v>1</v>
       </c>
       <c r="Q88" s="4" t="str">
-        <f>IF(ISBLANK(Y88), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -6112,11 +6112,11 @@
         <v>274</v>
       </c>
       <c r="G89" s="4">
-        <f>SUM(O89:W89)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q89" s="4" t="str">
-        <f>IF(ISBLANK(Y89), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T89" s="4">
@@ -6140,11 +6140,11 @@
         <v>444</v>
       </c>
       <c r="G90" s="4">
-        <f>SUM(O90:W90)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q90" s="4" t="str">
-        <f>IF(ISBLANK(Y90), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T90" s="4">
@@ -6168,14 +6168,14 @@
         <v>230</v>
       </c>
       <c r="G91" s="4">
-        <f>SUM(O91:W91)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P91" s="4">
         <v>1</v>
       </c>
       <c r="Q91" s="4" t="str">
-        <f>IF(ISBLANK(Y91), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -6193,11 +6193,11 @@
         <v>380</v>
       </c>
       <c r="G92" s="4">
-        <f>SUM(O92:W92)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q92" s="4" t="str">
-        <f>IF(ISBLANK(Y92), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="W92" s="4">
@@ -6218,11 +6218,11 @@
         <v>101</v>
       </c>
       <c r="G93" s="4">
-        <f>SUM(O93:W93)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q93" s="4" t="str">
-        <f>IF(ISBLANK(Y93), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="W93" s="4">
@@ -6243,11 +6243,11 @@
         <v>128</v>
       </c>
       <c r="G94" s="4">
-        <f>SUM(O94:W94)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q94" s="4" t="str">
-        <f>IF(ISBLANK(Y94), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="W94" s="4">
@@ -6268,14 +6268,14 @@
         <v>288</v>
       </c>
       <c r="G95" s="4">
-        <f>SUM(O95:W95)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O95" s="4">
         <v>1</v>
       </c>
       <c r="Q95" s="4" t="str">
-        <f>IF(ISBLANK(Y95), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -6293,11 +6293,11 @@
         <v>64</v>
       </c>
       <c r="G96" s="4">
-        <f>SUM(O96:W96)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q96" s="4" t="str">
-        <f>IF(ISBLANK(Y96), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="V96" s="4">
@@ -6318,14 +6318,14 @@
         <v>347</v>
       </c>
       <c r="G97" s="4">
-        <f>SUM(O97:W97)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O97" s="4">
         <v>1</v>
       </c>
       <c r="Q97" s="4" t="str">
-        <f>IF(ISBLANK(Y97), "", 1)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -6343,11 +6343,11 @@
         <v>367</v>
       </c>
       <c r="G98" s="4">
-        <f>SUM(O98:W98)</f>
+        <f t="shared" ref="G98:G129" si="6">SUM(O98:W98)</f>
         <v>1</v>
       </c>
       <c r="Q98" s="4" t="str">
-        <f>IF(ISBLANK(Y98), "", 1)</f>
+        <f t="shared" ref="Q98:Q110" si="7">IF(ISBLANK(Y98), "", 1)</f>
         <v/>
       </c>
       <c r="R98" s="4">
@@ -6368,14 +6368,14 @@
         <v>40</v>
       </c>
       <c r="G99" s="4">
-        <f>SUM(O99:W99)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O99" s="4">
         <v>1</v>
       </c>
       <c r="Q99" s="4" t="str">
-        <f>IF(ISBLANK(Y99), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6393,11 +6393,11 @@
         <v>77</v>
       </c>
       <c r="G100" s="4">
-        <f>SUM(O100:W100)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q100" s="4" t="str">
-        <f>IF(ISBLANK(Y100), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="V100" s="4">
@@ -6418,11 +6418,11 @@
         <v>121</v>
       </c>
       <c r="G101" s="4">
-        <f>SUM(O101:W101)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q101" s="4" t="str">
-        <f>IF(ISBLANK(Y101), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="W101" s="4">
@@ -6443,11 +6443,11 @@
         <v>104</v>
       </c>
       <c r="G102" s="4">
-        <f>SUM(O102:W102)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q102" s="4" t="str">
-        <f>IF(ISBLANK(Y102), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="W102" s="4">
@@ -6471,11 +6471,11 @@
         <v>125</v>
       </c>
       <c r="G103" s="4">
-        <f>SUM(O103:W103)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q103" s="4" t="str">
-        <f>IF(ISBLANK(Y103), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="W103" s="4">
@@ -6496,14 +6496,14 @@
         <v>306</v>
       </c>
       <c r="G104" s="4">
-        <f>SUM(O104:W104)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O104" s="4">
         <v>1</v>
       </c>
       <c r="Q104" s="4" t="str">
-        <f>IF(ISBLANK(Y104), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6521,11 +6521,11 @@
         <v>334</v>
       </c>
       <c r="G105" s="4">
-        <f>SUM(O105:W105)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q105" s="4" t="str">
-        <f>IF(ISBLANK(Y105), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="V105" s="4">
@@ -6546,14 +6546,14 @@
         <v>343</v>
       </c>
       <c r="G106" s="4">
-        <f>SUM(O106:W106)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P106" s="4">
         <v>1</v>
       </c>
       <c r="Q106" s="4" t="str">
-        <f>IF(ISBLANK(Y106), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6571,14 +6571,14 @@
         <v>252</v>
       </c>
       <c r="G107" s="4">
-        <f>SUM(O107:W107)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P107" s="4">
         <v>1</v>
       </c>
       <c r="Q107" s="4" t="str">
-        <f>IF(ISBLANK(Y107), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -6596,11 +6596,11 @@
         <v>375</v>
       </c>
       <c r="G108" s="4">
-        <f>SUM(O108:W108)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q108" s="4" t="str">
-        <f>IF(ISBLANK(Y108), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="R108" s="4">
@@ -6621,11 +6621,11 @@
         <v>331</v>
       </c>
       <c r="G109" s="4">
-        <f>SUM(O109:W109)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q109" s="4" t="str">
-        <f>IF(ISBLANK(Y109), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="T109" s="4">
@@ -6643,11 +6643,11 @@
         <v>338</v>
       </c>
       <c r="G110" s="4">
-        <f>SUM(O110:W110)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q110" s="4" t="str">
-        <f>IF(ISBLANK(Y110), "", 1)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="T110" s="4">
@@ -6671,7 +6671,7 @@
         <v>512</v>
       </c>
       <c r="G111" s="4">
-        <f>SUM(O111:W111)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H111" s="4" t="s">
@@ -6701,7 +6701,7 @@
         <v>510</v>
       </c>
       <c r="G112" s="4">
-        <f>SUM(O112:W112)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K112" s="23" t="s">
@@ -6728,11 +6728,11 @@
         <v>92</v>
       </c>
       <c r="G113" s="4">
-        <f>SUM(O113:W113)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q113" s="4" t="str">
-        <f>IF(ISBLANK(Y113), "", 1)</f>
+        <f t="shared" ref="Q113:Q125" si="8">IF(ISBLANK(Y113), "", 1)</f>
         <v/>
       </c>
     </row>
@@ -6750,11 +6750,11 @@
         <v>208</v>
       </c>
       <c r="G114" s="4">
-        <f>SUM(O114:W114)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q114" s="4" t="str">
-        <f>IF(ISBLANK(Y114), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -6772,11 +6772,11 @@
         <v>204</v>
       </c>
       <c r="G115" s="4">
-        <f>SUM(O115:W115)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q115" s="4" t="str">
-        <f>IF(ISBLANK(Y115), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -6794,14 +6794,14 @@
         <v>379</v>
       </c>
       <c r="G116" s="4">
-        <f>SUM(O116:W116)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O116" s="4">
         <v>-1</v>
       </c>
       <c r="Q116" s="4" t="str">
-        <f>IF(ISBLANK(Y116), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="T116" s="4">
@@ -6822,11 +6822,11 @@
         <v>198</v>
       </c>
       <c r="G117" s="4">
-        <f>SUM(O117:W117)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q117" s="4" t="str">
-        <f>IF(ISBLANK(Y117), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -6847,11 +6847,11 @@
         <v>244</v>
       </c>
       <c r="G118" s="4">
-        <f>SUM(O118:W118)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q118" s="4" t="str">
-        <f>IF(ISBLANK(Y118), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -6872,11 +6872,11 @@
         <v>257</v>
       </c>
       <c r="G119" s="4">
-        <f>SUM(O119:W119)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q119" s="4" t="str">
-        <f>IF(ISBLANK(Y119), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -6894,11 +6894,11 @@
         <v>297</v>
       </c>
       <c r="G120" s="4">
-        <f>SUM(O120:W120)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q120" s="4" t="str">
-        <f>IF(ISBLANK(Y120), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -6916,11 +6916,11 @@
         <v>234</v>
       </c>
       <c r="G121" s="4">
-        <f>SUM(O121:W121)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q121" s="4" t="str">
-        <f>IF(ISBLANK(Y121), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -6941,11 +6941,11 @@
         <v>428</v>
       </c>
       <c r="G122" s="4">
-        <f>SUM(O122:W122)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q122" s="4" t="str">
-        <f>IF(ISBLANK(Y122), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -6966,11 +6966,11 @@
         <v>295</v>
       </c>
       <c r="G123" s="4">
-        <f>SUM(O123:W123)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q123" s="4" t="str">
-        <f>IF(ISBLANK(Y123), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -6991,11 +6991,11 @@
         <v>271</v>
       </c>
       <c r="G124" s="4">
-        <f>SUM(O124:W124)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q124" s="4" t="str">
-        <f>IF(ISBLANK(Y124), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -7016,11 +7016,11 @@
         <v>66</v>
       </c>
       <c r="G125" s="4">
-        <f>SUM(O125:W125)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q125" s="4" t="str">
-        <f>IF(ISBLANK(Y125), "", 1)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -7038,7 +7038,7 @@
         <v>506</v>
       </c>
       <c r="G126" s="4">
-        <f>SUM(O126:W126)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Y126" t="s">
@@ -7062,11 +7062,11 @@
         <v>217</v>
       </c>
       <c r="G127" s="4">
-        <f>SUM(O127:W127)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q127" s="4" t="str">
-        <f>IF(ISBLANK(Y127), "", 1)</f>
+        <f t="shared" ref="Q127:Q139" si="9">IF(ISBLANK(Y127), "", 1)</f>
         <v/>
       </c>
     </row>
@@ -7084,11 +7084,11 @@
         <v>263</v>
       </c>
       <c r="G128" s="4">
-        <f>SUM(O128:W128)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q128" s="4" t="str">
-        <f>IF(ISBLANK(Y128), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7106,11 +7106,11 @@
         <v>324</v>
       </c>
       <c r="G129" s="4">
-        <f>SUM(O129:W129)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q129" s="4" t="str">
-        <f>IF(ISBLANK(Y129), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7128,11 +7128,11 @@
         <v>328</v>
       </c>
       <c r="G130" s="4">
-        <f>SUM(O130:W130)</f>
+        <f t="shared" ref="G130:G139" si="10">SUM(O130:W130)</f>
         <v>0</v>
       </c>
       <c r="Q130" s="4" t="str">
-        <f>IF(ISBLANK(Y130), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7150,11 +7150,11 @@
         <v>345</v>
       </c>
       <c r="G131" s="4">
-        <f>SUM(O131:W131)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q131" s="4" t="str">
-        <f>IF(ISBLANK(Y131), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7169,11 +7169,11 @@
         <v>340</v>
       </c>
       <c r="G132" s="4">
-        <f>SUM(O132:W132)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q132" s="4" t="str">
-        <f>IF(ISBLANK(Y132), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7191,11 +7191,11 @@
         <v>320</v>
       </c>
       <c r="G133" s="4">
-        <f>SUM(O133:W133)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q133" s="4" t="str">
-        <f>IF(ISBLANK(Y133), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7210,11 +7210,11 @@
         <v>200</v>
       </c>
       <c r="G134" s="4">
-        <f>SUM(O134:W134)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q134" s="4" t="str">
-        <f>IF(ISBLANK(Y134), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7229,11 +7229,11 @@
         <v>381</v>
       </c>
       <c r="G135" s="4">
-        <f>SUM(O135:W135)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q135" s="4" t="str">
-        <f>IF(ISBLANK(Y135), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7248,11 +7248,11 @@
         <v>310</v>
       </c>
       <c r="G136" s="4">
-        <f>SUM(O136:W136)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q136" s="4" t="str">
-        <f>IF(ISBLANK(Y136), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7270,11 +7270,11 @@
         <v>301</v>
       </c>
       <c r="G137" s="4">
-        <f>SUM(O137:W137)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q137" s="4" t="str">
-        <f>IF(ISBLANK(Y137), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7289,11 +7289,11 @@
         <v>292</v>
       </c>
       <c r="G138" s="4">
-        <f>SUM(O138:W138)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q138" s="4" t="str">
-        <f>IF(ISBLANK(Y138), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -7308,11 +7308,11 @@
         <v>336</v>
       </c>
       <c r="G139" s="4">
-        <f>SUM(O139:W139)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q139" s="4" t="str">
-        <f>IF(ISBLANK(Y139), "", 1)</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>

</xml_diff>